<commit_message>
solutions with error < 0.1
</commit_message>
<xml_diff>
--- a/tiny-gp/output/f4_2_data.xlsx
+++ b/tiny-gp/output/f4_2_data.xlsx
@@ -99,7 +99,7 @@
         <v>-30.0</v>
       </c>
       <c r="D2" s="0">
-        <f>((A2*(B2/B2))+(B2+B2))</f>
+        <f>((B2+B2)+A2)</f>
       </c>
     </row>
     <row r="3">
@@ -113,7 +113,7 @@
         <v>-25.555555555555557</v>
       </c>
       <c r="D3" s="0">
-        <f>((A3*(B3/B3))+(B3+B3))</f>
+        <f>((B3+B3)+A3)</f>
       </c>
     </row>
     <row r="4">
@@ -127,7 +127,7 @@
         <v>-21.11111111111111</v>
       </c>
       <c r="D4" s="0">
-        <f>((A4*(B4/B4))+(B4+B4))</f>
+        <f>((B4+B4)+A4)</f>
       </c>
     </row>
     <row r="5">
@@ -141,7 +141,7 @@
         <v>-16.666666666666664</v>
       </c>
       <c r="D5" s="0">
-        <f>((A5*(B5/B5))+(B5+B5))</f>
+        <f>((B5+B5)+A5)</f>
       </c>
     </row>
     <row r="6">
@@ -155,7 +155,7 @@
         <v>-12.222222222222221</v>
       </c>
       <c r="D6" s="0">
-        <f>((A6*(B6/B6))+(B6+B6))</f>
+        <f>((B6+B6)+A6)</f>
       </c>
     </row>
     <row r="7">
@@ -169,7 +169,7 @@
         <v>-7.777777777777779</v>
       </c>
       <c r="D7" s="0">
-        <f>((A7*(B7/B7))+(B7+B7))</f>
+        <f>((B7+B7)+A7)</f>
       </c>
     </row>
     <row r="8">
@@ -183,7 +183,7 @@
         <v>-3.333333333333332</v>
       </c>
       <c r="D8" s="0">
-        <f>((A8*(B8/B8))+(B8+B8))</f>
+        <f>((B8+B8)+A8)</f>
       </c>
     </row>
     <row r="9">
@@ -197,7 +197,7 @@
         <v>1.1111111111111143</v>
       </c>
       <c r="D9" s="0">
-        <f>((A9*(B9/B9))+(B9+B9))</f>
+        <f>((B9+B9)+A9)</f>
       </c>
     </row>
     <row r="10">
@@ -211,7 +211,7 @@
         <v>5.555555555555557</v>
       </c>
       <c r="D10" s="0">
-        <f>((A10*(B10/B10))+(B10+B10))</f>
+        <f>((B10+B10)+A10)</f>
       </c>
     </row>
     <row r="11">
@@ -225,7 +225,7 @@
         <v>10.0</v>
       </c>
       <c r="D11" s="0">
-        <f>((A11*(B11/B11))+(B11+B11))</f>
+        <f>((B11+B11)+A11)</f>
       </c>
     </row>
     <row r="12">
@@ -239,7 +239,7 @@
         <v>-27.77777777777778</v>
       </c>
       <c r="D12" s="0">
-        <f>((A12*(B12/B12))+(B12+B12))</f>
+        <f>((B12+B12)+A12)</f>
       </c>
     </row>
     <row r="13">
@@ -253,7 +253,7 @@
         <v>-23.333333333333332</v>
       </c>
       <c r="D13" s="0">
-        <f>((A13*(B13/B13))+(B13+B13))</f>
+        <f>((B13+B13)+A13)</f>
       </c>
     </row>
     <row r="14">
@@ -267,7 +267,7 @@
         <v>-18.88888888888889</v>
       </c>
       <c r="D14" s="0">
-        <f>((A14*(B14/B14))+(B14+B14))</f>
+        <f>((B14+B14)+A14)</f>
       </c>
     </row>
     <row r="15">
@@ -281,7 +281,7 @@
         <v>-14.444444444444443</v>
       </c>
       <c r="D15" s="0">
-        <f>((A15*(B15/B15))+(B15+B15))</f>
+        <f>((B15+B15)+A15)</f>
       </c>
     </row>
     <row r="16">
@@ -295,7 +295,7 @@
         <v>-10.0</v>
       </c>
       <c r="D16" s="0">
-        <f>((A16*(B16/B16))+(B16+B16))</f>
+        <f>((B16+B16)+A16)</f>
       </c>
     </row>
     <row r="17">
@@ -309,7 +309,7 @@
         <v>-5.555555555555556</v>
       </c>
       <c r="D17" s="0">
-        <f>((A17*(B17/B17))+(B17+B17))</f>
+        <f>((B17+B17)+A17)</f>
       </c>
     </row>
     <row r="18">
@@ -323,7 +323,7 @@
         <v>-1.1111111111111098</v>
       </c>
       <c r="D18" s="0">
-        <f>((A18*(B18/B18))+(B18+B18))</f>
+        <f>((B18+B18)+A18)</f>
       </c>
     </row>
     <row r="19">
@@ -337,7 +337,7 @@
         <v>3.3333333333333366</v>
       </c>
       <c r="D19" s="0">
-        <f>((A19*(B19/B19))+(B19+B19))</f>
+        <f>((B19+B19)+A19)</f>
       </c>
     </row>
     <row r="20">
@@ -351,7 +351,7 @@
         <v>7.7777777777777795</v>
       </c>
       <c r="D20" s="0">
-        <f>((A20*(B20/B20))+(B20+B20))</f>
+        <f>((B20+B20)+A20)</f>
       </c>
     </row>
     <row r="21">
@@ -365,7 +365,7 @@
         <v>12.222222222222221</v>
       </c>
       <c r="D21" s="0">
-        <f>((A21*(B21/B21))+(B21+B21))</f>
+        <f>((B21+B21)+A21)</f>
       </c>
     </row>
     <row r="22">
@@ -379,7 +379,7 @@
         <v>-25.555555555555557</v>
       </c>
       <c r="D22" s="0">
-        <f>((A22*(B22/B22))+(B22+B22))</f>
+        <f>((B22+B22)+A22)</f>
       </c>
     </row>
     <row r="23">
@@ -393,7 +393,7 @@
         <v>-21.11111111111111</v>
       </c>
       <c r="D23" s="0">
-        <f>((A23*(B23/B23))+(B23+B23))</f>
+        <f>((B23+B23)+A23)</f>
       </c>
     </row>
     <row r="24">
@@ -407,7 +407,7 @@
         <v>-16.666666666666664</v>
       </c>
       <c r="D24" s="0">
-        <f>((A24*(B24/B24))+(B24+B24))</f>
+        <f>((B24+B24)+A24)</f>
       </c>
     </row>
     <row r="25">
@@ -421,7 +421,7 @@
         <v>-12.222222222222221</v>
       </c>
       <c r="D25" s="0">
-        <f>((A25*(B25/B25))+(B25+B25))</f>
+        <f>((B25+B25)+A25)</f>
       </c>
     </row>
     <row r="26">
@@ -435,7 +435,7 @@
         <v>-7.777777777777777</v>
       </c>
       <c r="D26" s="0">
-        <f>((A26*(B26/B26))+(B26+B26))</f>
+        <f>((B26+B26)+A26)</f>
       </c>
     </row>
     <row r="27">
@@ -449,7 +449,7 @@
         <v>-3.333333333333334</v>
       </c>
       <c r="D27" s="0">
-        <f>((A27*(B27/B27))+(B27+B27))</f>
+        <f>((B27+B27)+A27)</f>
       </c>
     </row>
     <row r="28">
@@ -463,7 +463,7 @@
         <v>1.1111111111111125</v>
       </c>
       <c r="D28" s="0">
-        <f>((A28*(B28/B28))+(B28+B28))</f>
+        <f>((B28+B28)+A28)</f>
       </c>
     </row>
     <row r="29">
@@ -477,7 +477,7 @@
         <v>5.555555555555559</v>
       </c>
       <c r="D29" s="0">
-        <f>((A29*(B29/B29))+(B29+B29))</f>
+        <f>((B29+B29)+A29)</f>
       </c>
     </row>
     <row r="30">
@@ -491,7 +491,7 @@
         <v>10.000000000000002</v>
       </c>
       <c r="D30" s="0">
-        <f>((A30*(B30/B30))+(B30+B30))</f>
+        <f>((B30+B30)+A30)</f>
       </c>
     </row>
     <row r="31">
@@ -505,7 +505,7 @@
         <v>14.444444444444445</v>
       </c>
       <c r="D31" s="0">
-        <f>((A31*(B31/B31))+(B31+B31))</f>
+        <f>((B31+B31)+A31)</f>
       </c>
     </row>
     <row r="32">
@@ -519,7 +519,7 @@
         <v>-23.333333333333332</v>
       </c>
       <c r="D32" s="0">
-        <f>((A32*(B32/B32))+(B32+B32))</f>
+        <f>((B32+B32)+A32)</f>
       </c>
     </row>
     <row r="33">
@@ -533,7 +533,7 @@
         <v>-18.88888888888889</v>
       </c>
       <c r="D33" s="0">
-        <f>((A33*(B33/B33))+(B33+B33))</f>
+        <f>((B33+B33)+A33)</f>
       </c>
     </row>
     <row r="34">
@@ -547,7 +547,7 @@
         <v>-14.444444444444443</v>
       </c>
       <c r="D34" s="0">
-        <f>((A34*(B34/B34))+(B34+B34))</f>
+        <f>((B34+B34)+A34)</f>
       </c>
     </row>
     <row r="35">
@@ -561,7 +561,7 @@
         <v>-10.0</v>
       </c>
       <c r="D35" s="0">
-        <f>((A35*(B35/B35))+(B35+B35))</f>
+        <f>((B35+B35)+A35)</f>
       </c>
     </row>
     <row r="36">
@@ -575,7 +575,7 @@
         <v>-5.5555555555555545</v>
       </c>
       <c r="D36" s="0">
-        <f>((A36*(B36/B36))+(B36+B36))</f>
+        <f>((B36+B36)+A36)</f>
       </c>
     </row>
     <row r="37">
@@ -589,7 +589,7 @@
         <v>-1.1111111111111116</v>
       </c>
       <c r="D37" s="0">
-        <f>((A37*(B37/B37))+(B37+B37))</f>
+        <f>((B37+B37)+A37)</f>
       </c>
     </row>
     <row r="38">
@@ -603,7 +603,7 @@
         <v>3.333333333333335</v>
       </c>
       <c r="D38" s="0">
-        <f>((A38*(B38/B38))+(B38+B38))</f>
+        <f>((B38+B38)+A38)</f>
       </c>
     </row>
     <row r="39">
@@ -617,7 +617,7 @@
         <v>7.777777777777781</v>
       </c>
       <c r="D39" s="0">
-        <f>((A39*(B39/B39))+(B39+B39))</f>
+        <f>((B39+B39)+A39)</f>
       </c>
     </row>
     <row r="40">
@@ -631,7 +631,7 @@
         <v>12.222222222222225</v>
       </c>
       <c r="D40" s="0">
-        <f>((A40*(B40/B40))+(B40+B40))</f>
+        <f>((B40+B40)+A40)</f>
       </c>
     </row>
     <row r="41">
@@ -645,7 +645,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="D41" s="0">
-        <f>((A41*(B41/B41))+(B41+B41))</f>
+        <f>((B41+B41)+A41)</f>
       </c>
     </row>
     <row r="42">
@@ -659,7 +659,7 @@
         <v>-21.11111111111111</v>
       </c>
       <c r="D42" s="0">
-        <f>((A42*(B42/B42))+(B42+B42))</f>
+        <f>((B42+B42)+A42)</f>
       </c>
     </row>
     <row r="43">
@@ -673,7 +673,7 @@
         <v>-16.666666666666664</v>
       </c>
       <c r="D43" s="0">
-        <f>((A43*(B43/B43))+(B43+B43))</f>
+        <f>((B43+B43)+A43)</f>
       </c>
     </row>
     <row r="44">
@@ -687,7 +687,7 @@
         <v>-12.222222222222221</v>
       </c>
       <c r="D44" s="0">
-        <f>((A44*(B44/B44))+(B44+B44))</f>
+        <f>((B44+B44)+A44)</f>
       </c>
     </row>
     <row r="45">
@@ -701,7 +701,7 @@
         <v>-7.777777777777777</v>
       </c>
       <c r="D45" s="0">
-        <f>((A45*(B45/B45))+(B45+B45))</f>
+        <f>((B45+B45)+A45)</f>
       </c>
     </row>
     <row r="46">
@@ -715,7 +715,7 @@
         <v>-3.333333333333332</v>
       </c>
       <c r="D46" s="0">
-        <f>((A46*(B46/B46))+(B46+B46))</f>
+        <f>((B46+B46)+A46)</f>
       </c>
     </row>
     <row r="47">
@@ -729,7 +729,7 @@
         <v>1.1111111111111107</v>
       </c>
       <c r="D47" s="0">
-        <f>((A47*(B47/B47))+(B47+B47))</f>
+        <f>((B47+B47)+A47)</f>
       </c>
     </row>
     <row r="48">
@@ -743,7 +743,7 @@
         <v>5.555555555555557</v>
       </c>
       <c r="D48" s="0">
-        <f>((A48*(B48/B48))+(B48+B48))</f>
+        <f>((B48+B48)+A48)</f>
       </c>
     </row>
     <row r="49">
@@ -757,7 +757,7 @@
         <v>10.000000000000004</v>
       </c>
       <c r="D49" s="0">
-        <f>((A49*(B49/B49))+(B49+B49))</f>
+        <f>((B49+B49)+A49)</f>
       </c>
     </row>
     <row r="50">
@@ -771,7 +771,7 @@
         <v>14.444444444444446</v>
       </c>
       <c r="D50" s="0">
-        <f>((A50*(B50/B50))+(B50+B50))</f>
+        <f>((B50+B50)+A50)</f>
       </c>
     </row>
     <row r="51">
@@ -785,7 +785,7 @@
         <v>18.88888888888889</v>
       </c>
       <c r="D51" s="0">
-        <f>((A51*(B51/B51))+(B51+B51))</f>
+        <f>((B51+B51)+A51)</f>
       </c>
     </row>
     <row r="52">
@@ -799,7 +799,7 @@
         <v>-18.88888888888889</v>
       </c>
       <c r="D52" s="0">
-        <f>((A52*(B52/B52))+(B52+B52))</f>
+        <f>((B52+B52)+A52)</f>
       </c>
     </row>
     <row r="53">
@@ -813,7 +813,7 @@
         <v>-14.444444444444445</v>
       </c>
       <c r="D53" s="0">
-        <f>((A53*(B53/B53))+(B53+B53))</f>
+        <f>((B53+B53)+A53)</f>
       </c>
     </row>
     <row r="54">
@@ -827,7 +827,7 @@
         <v>-10.0</v>
       </c>
       <c r="D54" s="0">
-        <f>((A54*(B54/B54))+(B54+B54))</f>
+        <f>((B54+B54)+A54)</f>
       </c>
     </row>
     <row r="55">
@@ -841,7 +841,7 @@
         <v>-5.555555555555555</v>
       </c>
       <c r="D55" s="0">
-        <f>((A55*(B55/B55))+(B55+B55))</f>
+        <f>((B55+B55)+A55)</f>
       </c>
     </row>
     <row r="56">
@@ -855,7 +855,7 @@
         <v>-1.1111111111111107</v>
       </c>
       <c r="D56" s="0">
-        <f>((A56*(B56/B56))+(B56+B56))</f>
+        <f>((B56+B56)+A56)</f>
       </c>
     </row>
     <row r="57">
@@ -869,7 +869,7 @@
         <v>3.333333333333332</v>
       </c>
       <c r="D57" s="0">
-        <f>((A57*(B57/B57))+(B57+B57))</f>
+        <f>((B57+B57)+A57)</f>
       </c>
     </row>
     <row r="58">
@@ -883,7 +883,7 @@
         <v>7.777777777777779</v>
       </c>
       <c r="D58" s="0">
-        <f>((A58*(B58/B58))+(B58+B58))</f>
+        <f>((B58+B58)+A58)</f>
       </c>
     </row>
     <row r="59">
@@ -897,7 +897,7 @@
         <v>12.222222222222225</v>
       </c>
       <c r="D59" s="0">
-        <f>((A59*(B59/B59))+(B59+B59))</f>
+        <f>((B59+B59)+A59)</f>
       </c>
     </row>
     <row r="60">
@@ -911,7 +911,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="D60" s="0">
-        <f>((A60*(B60/B60))+(B60+B60))</f>
+        <f>((B60+B60)+A60)</f>
       </c>
     </row>
     <row r="61">
@@ -925,7 +925,7 @@
         <v>21.11111111111111</v>
       </c>
       <c r="D61" s="0">
-        <f>((A61*(B61/B61))+(B61+B61))</f>
+        <f>((B61+B61)+A61)</f>
       </c>
     </row>
     <row r="62">
@@ -939,7 +939,7 @@
         <v>-16.666666666666664</v>
       </c>
       <c r="D62" s="0">
-        <f>((A62*(B62/B62))+(B62+B62))</f>
+        <f>((B62+B62)+A62)</f>
       </c>
     </row>
     <row r="63">
@@ -953,7 +953,7 @@
         <v>-12.222222222222221</v>
       </c>
       <c r="D63" s="0">
-        <f>((A63*(B63/B63))+(B63+B63))</f>
+        <f>((B63+B63)+A63)</f>
       </c>
     </row>
     <row r="64">
@@ -967,7 +967,7 @@
         <v>-7.777777777777777</v>
       </c>
       <c r="D64" s="0">
-        <f>((A64*(B64/B64))+(B64+B64))</f>
+        <f>((B64+B64)+A64)</f>
       </c>
     </row>
     <row r="65">
@@ -981,7 +981,7 @@
         <v>-3.333333333333332</v>
       </c>
       <c r="D65" s="0">
-        <f>((A65*(B65/B65))+(B65+B65))</f>
+        <f>((B65+B65)+A65)</f>
       </c>
     </row>
     <row r="66">
@@ -995,7 +995,7 @@
         <v>1.1111111111111125</v>
       </c>
       <c r="D66" s="0">
-        <f>((A66*(B66/B66))+(B66+B66))</f>
+        <f>((B66+B66)+A66)</f>
       </c>
     </row>
     <row r="67">
@@ -1009,7 +1009,7 @@
         <v>5.555555555555555</v>
       </c>
       <c r="D67" s="0">
-        <f>((A67*(B67/B67))+(B67+B67))</f>
+        <f>((B67+B67)+A67)</f>
       </c>
     </row>
     <row r="68">
@@ -1023,7 +1023,7 @@
         <v>10.000000000000002</v>
       </c>
       <c r="D68" s="0">
-        <f>((A68*(B68/B68))+(B68+B68))</f>
+        <f>((B68+B68)+A68)</f>
       </c>
     </row>
     <row r="69">
@@ -1037,7 +1037,7 @@
         <v>14.444444444444448</v>
       </c>
       <c r="D69" s="0">
-        <f>((A69*(B69/B69))+(B69+B69))</f>
+        <f>((B69+B69)+A69)</f>
       </c>
     </row>
     <row r="70">
@@ -1051,7 +1051,7 @@
         <v>18.888888888888893</v>
       </c>
       <c r="D70" s="0">
-        <f>((A70*(B70/B70))+(B70+B70))</f>
+        <f>((B70+B70)+A70)</f>
       </c>
     </row>
     <row r="71">
@@ -1065,7 +1065,7 @@
         <v>23.333333333333336</v>
       </c>
       <c r="D71" s="0">
-        <f>((A71*(B71/B71))+(B71+B71))</f>
+        <f>((B71+B71)+A71)</f>
       </c>
     </row>
     <row r="72">
@@ -1079,7 +1079,7 @@
         <v>-14.444444444444443</v>
       </c>
       <c r="D72" s="0">
-        <f>((A72*(B72/B72))+(B72+B72))</f>
+        <f>((B72+B72)+A72)</f>
       </c>
     </row>
     <row r="73">
@@ -1093,7 +1093,7 @@
         <v>-9.999999999999998</v>
       </c>
       <c r="D73" s="0">
-        <f>((A73*(B73/B73))+(B73+B73))</f>
+        <f>((B73+B73)+A73)</f>
       </c>
     </row>
     <row r="74">
@@ -1107,7 +1107,7 @@
         <v>-5.555555555555554</v>
       </c>
       <c r="D74" s="0">
-        <f>((A74*(B74/B74))+(B74+B74))</f>
+        <f>((B74+B74)+A74)</f>
       </c>
     </row>
     <row r="75">
@@ -1121,7 +1121,7 @@
         <v>-1.111111111111109</v>
       </c>
       <c r="D75" s="0">
-        <f>((A75*(B75/B75))+(B75+B75))</f>
+        <f>((B75+B75)+A75)</f>
       </c>
     </row>
     <row r="76">
@@ -1135,7 +1135,7 @@
         <v>3.3333333333333357</v>
       </c>
       <c r="D76" s="0">
-        <f>((A76*(B76/B76))+(B76+B76))</f>
+        <f>((B76+B76)+A76)</f>
       </c>
     </row>
     <row r="77">
@@ -1149,7 +1149,7 @@
         <v>7.777777777777779</v>
       </c>
       <c r="D77" s="0">
-        <f>((A77*(B77/B77))+(B77+B77))</f>
+        <f>((B77+B77)+A77)</f>
       </c>
     </row>
     <row r="78">
@@ -1163,7 +1163,7 @@
         <v>12.222222222222225</v>
       </c>
       <c r="D78" s="0">
-        <f>((A78*(B78/B78))+(B78+B78))</f>
+        <f>((B78+B78)+A78)</f>
       </c>
     </row>
     <row r="79">
@@ -1177,7 +1177,7 @@
         <v>16.66666666666667</v>
       </c>
       <c r="D79" s="0">
-        <f>((A79*(B79/B79))+(B79+B79))</f>
+        <f>((B79+B79)+A79)</f>
       </c>
     </row>
     <row r="80">
@@ -1191,7 +1191,7 @@
         <v>21.111111111111114</v>
       </c>
       <c r="D80" s="0">
-        <f>((A80*(B80/B80))+(B80+B80))</f>
+        <f>((B80+B80)+A80)</f>
       </c>
     </row>
     <row r="81">
@@ -1205,7 +1205,7 @@
         <v>25.555555555555557</v>
       </c>
       <c r="D81" s="0">
-        <f>((A81*(B81/B81))+(B81+B81))</f>
+        <f>((B81+B81)+A81)</f>
       </c>
     </row>
     <row r="82">
@@ -1219,7 +1219,7 @@
         <v>-12.222222222222221</v>
       </c>
       <c r="D82" s="0">
-        <f>((A82*(B82/B82))+(B82+B82))</f>
+        <f>((B82+B82)+A82)</f>
       </c>
     </row>
     <row r="83">
@@ -1233,7 +1233,7 @@
         <v>-7.777777777777777</v>
       </c>
       <c r="D83" s="0">
-        <f>((A83*(B83/B83))+(B83+B83))</f>
+        <f>((B83+B83)+A83)</f>
       </c>
     </row>
     <row r="84">
@@ -1247,7 +1247,7 @@
         <v>-3.333333333333332</v>
       </c>
       <c r="D84" s="0">
-        <f>((A84*(B84/B84))+(B84+B84))</f>
+        <f>((B84+B84)+A84)</f>
       </c>
     </row>
     <row r="85">
@@ -1261,7 +1261,7 @@
         <v>1.1111111111111125</v>
       </c>
       <c r="D85" s="0">
-        <f>((A85*(B85/B85))+(B85+B85))</f>
+        <f>((B85+B85)+A85)</f>
       </c>
     </row>
     <row r="86">
@@ -1275,7 +1275,7 @@
         <v>5.555555555555557</v>
       </c>
       <c r="D86" s="0">
-        <f>((A86*(B86/B86))+(B86+B86))</f>
+        <f>((B86+B86)+A86)</f>
       </c>
     </row>
     <row r="87">
@@ -1289,7 +1289,7 @@
         <v>10.0</v>
       </c>
       <c r="D87" s="0">
-        <f>((A87*(B87/B87))+(B87+B87))</f>
+        <f>((B87+B87)+A87)</f>
       </c>
     </row>
     <row r="88">
@@ -1303,7 +1303,7 @@
         <v>14.444444444444446</v>
       </c>
       <c r="D88" s="0">
-        <f>((A88*(B88/B88))+(B88+B88))</f>
+        <f>((B88+B88)+A88)</f>
       </c>
     </row>
     <row r="89">
@@ -1317,7 +1317,7 @@
         <v>18.888888888888893</v>
       </c>
       <c r="D89" s="0">
-        <f>((A89*(B89/B89))+(B89+B89))</f>
+        <f>((B89+B89)+A89)</f>
       </c>
     </row>
     <row r="90">
@@ -1331,7 +1331,7 @@
         <v>23.333333333333336</v>
       </c>
       <c r="D90" s="0">
-        <f>((A90*(B90/B90))+(B90+B90))</f>
+        <f>((B90+B90)+A90)</f>
       </c>
     </row>
     <row r="91">
@@ -1345,7 +1345,7 @@
         <v>27.77777777777778</v>
       </c>
       <c r="D91" s="0">
-        <f>((A91*(B91/B91))+(B91+B91))</f>
+        <f>((B91+B91)+A91)</f>
       </c>
     </row>
     <row r="92">
@@ -1359,7 +1359,7 @@
         <v>-10.0</v>
       </c>
       <c r="D92" s="0">
-        <f>((A92*(B92/B92))+(B92+B92))</f>
+        <f>((B92+B92)+A92)</f>
       </c>
     </row>
     <row r="93">
@@ -1373,7 +1373,7 @@
         <v>-5.555555555555555</v>
       </c>
       <c r="D93" s="0">
-        <f>((A93*(B93/B93))+(B93+B93))</f>
+        <f>((B93+B93)+A93)</f>
       </c>
     </row>
     <row r="94">
@@ -1387,7 +1387,7 @@
         <v>-1.1111111111111107</v>
       </c>
       <c r="D94" s="0">
-        <f>((A94*(B94/B94))+(B94+B94))</f>
+        <f>((B94+B94)+A94)</f>
       </c>
     </row>
     <row r="95">
@@ -1401,7 +1401,7 @@
         <v>3.333333333333334</v>
       </c>
       <c r="D95" s="0">
-        <f>((A95*(B95/B95))+(B95+B95))</f>
+        <f>((B95+B95)+A95)</f>
       </c>
     </row>
     <row r="96">
@@ -1415,7 +1415,7 @@
         <v>7.777777777777779</v>
       </c>
       <c r="D96" s="0">
-        <f>((A96*(B96/B96))+(B96+B96))</f>
+        <f>((B96+B96)+A96)</f>
       </c>
     </row>
     <row r="97">
@@ -1429,7 +1429,7 @@
         <v>12.222222222222221</v>
       </c>
       <c r="D97" s="0">
-        <f>((A97*(B97/B97))+(B97+B97))</f>
+        <f>((B97+B97)+A97)</f>
       </c>
     </row>
     <row r="98">
@@ -1443,7 +1443,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="D98" s="0">
-        <f>((A98*(B98/B98))+(B98+B98))</f>
+        <f>((B98+B98)+A98)</f>
       </c>
     </row>
     <row r="99">
@@ -1457,7 +1457,7 @@
         <v>21.111111111111114</v>
       </c>
       <c r="D99" s="0">
-        <f>((A99*(B99/B99))+(B99+B99))</f>
+        <f>((B99+B99)+A99)</f>
       </c>
     </row>
     <row r="100">
@@ -1471,7 +1471,7 @@
         <v>25.555555555555557</v>
       </c>
       <c r="D100" s="0">
-        <f>((A100*(B100/B100))+(B100+B100))</f>
+        <f>((B100+B100)+A100)</f>
       </c>
     </row>
     <row r="101">
@@ -1485,7 +1485,7 @@
         <v>30.0</v>
       </c>
       <c r="D101" s="0">
-        <f>((A101*(B101/B101))+(B101+B101))</f>
+        <f>((B101+B101)+A101)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>